<commit_message>
benchmarking monolithic and distributed 2,3
</commit_message>
<xml_diff>
--- a/excel/data_layout_FINAL.xlsx
+++ b/excel/data_layout_FINAL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\natashaval\qubit-mapping-distributed-qc\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A697A55-DFD9-4422-9A6C-BF8F891CC74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07434D52-C340-4338-8579-ECDC7ADEA1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="57">
   <si>
     <t>layout</t>
   </si>
@@ -163,9 +163,6 @@
     <t>counts</t>
   </si>
   <si>
-    <t>t_vertical_4</t>
-  </si>
-  <si>
     <t>Benchmark [15]</t>
   </si>
   <si>
@@ -185,6 +182,30 @@
   </si>
   <si>
     <t>swap sabre - lookahead</t>
+  </si>
+  <si>
+    <t>Create STD</t>
+  </si>
+  <si>
+    <t>Methodology</t>
+  </si>
+  <si>
+    <t>line</t>
+  </si>
+  <si>
+    <t>grid</t>
+  </si>
+  <si>
+    <t>ring</t>
+  </si>
+  <si>
+    <t>full</t>
+  </si>
+  <si>
+    <t>t_horizontal</t>
+  </si>
+  <si>
+    <t>t_vertical</t>
   </si>
 </sst>
 </file>
@@ -222,7 +243,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,6 +259,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -278,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -290,9 +317,17 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,7 +426,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'n = 15'!$X$1</c:f>
+              <c:f>'n = 15'!$Z$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -402,7 +437,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent6"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -410,6 +445,63 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-9D3A-4D29-94E8-F68B28B76F2A}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-9D3A-4D29-94E8-F68B28B76F2A}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-9D3A-4D29-94E8-F68B28B76F2A}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -470,58 +562,76 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'n = 15'!$W$2:$W$8</c:f>
+              <c:f>'n = 15'!$Y$2:$Y$11</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>full_10_2</c:v>
+                  <c:v>line_5_4 (15)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>grid_4_5</c:v>
+                  <c:v>full_10_2 (15)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>grid_9_3</c:v>
+                  <c:v>full_7_3 (8)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>line_5_4</c:v>
+                  <c:v>grid_9_3 (15)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>ring_10_2</c:v>
+                  <c:v>grid_4_5 (15)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>t_horizontal_5_4</c:v>
+                  <c:v>ring_10_2 (15)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>t_vertical_4</c:v>
+                  <c:v>ring_7_3 (8)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ring_5_4 (6)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>t_horizontal_5_4 (15)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>t_vertical_5_4 (15)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'n = 15'!$X$2:$X$8</c:f>
+              <c:f>'n = 15'!$Z$2:$Z$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>61.018666666666668</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>53.36933333333333</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>41.216250000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65.397999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>66.805999999999997</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>65.397999999999996</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>61.018666666666668</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>48.56733333333333</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>33.421250000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22.03833333333333</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>69.309333333333328</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>70.554000000000002</c:v>
                 </c:pt>
               </c:numCache>
@@ -538,7 +648,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'n = 15'!$Y$1</c:f>
+              <c:f>'n = 15'!$AA$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -549,7 +659,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5"/>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -557,6 +667,63 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-9D3A-4D29-94E8-F68B28B76F2A}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-9D3A-4D29-94E8-F68B28B76F2A}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-9D3A-4D29-94E8-F68B28B76F2A}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -617,58 +784,76 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'n = 15'!$W$2:$W$8</c:f>
+              <c:f>'n = 15'!$Y$2:$Y$11</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>full_10_2</c:v>
+                  <c:v>line_5_4 (15)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>grid_4_5</c:v>
+                  <c:v>full_10_2 (15)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>grid_9_3</c:v>
+                  <c:v>full_7_3 (8)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>line_5_4</c:v>
+                  <c:v>grid_9_3 (15)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>ring_10_2</c:v>
+                  <c:v>grid_4_5 (15)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>t_horizontal_5_4</c:v>
+                  <c:v>ring_10_2 (15)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>t_vertical_4</c:v>
+                  <c:v>ring_7_3 (8)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ring_5_4 (6)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>t_horizontal_5_4 (15)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>t_vertical_5_4 (15)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'n = 15'!$Y$2:$Y$8</c:f>
+              <c:f>'n = 15'!$AA$2:$AA$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>34.147333333333336</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>27.371999999999996</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>19.568750000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.140666666666668</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>28.262666666666668</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>26.140666666666668</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>34.147333333333336</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>30.424666666666667</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>32.08</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38.961666666666666</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>28.018666666666665</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>32.405999999999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -1020,7 +1205,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'n = 15'!$T$40</c:f>
+              <c:f>'n = 15'!$V$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1096,7 +1281,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'n = 15'!$S$41:$S$50</c:f>
+              <c:f>'n = 15'!$U$41:$U$50</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1134,7 +1319,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'n = 15'!$T$41:$T$50</c:f>
+              <c:f>'n = 15'!$V$41:$V$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1182,7 +1367,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'n = 15'!$U$40</c:f>
+              <c:f>'n = 15'!$W$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1258,7 +1443,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'n = 15'!$S$41:$S$50</c:f>
+              <c:f>'n = 15'!$U$41:$U$50</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1296,7 +1481,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'n = 15'!$U$41:$U$50</c:f>
+              <c:f>'n = 15'!$W$41:$W$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1344,7 +1529,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'n = 15'!$V$40</c:f>
+              <c:f>'n = 15'!$X$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1420,7 +1605,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'n = 15'!$S$41:$S$50</c:f>
+              <c:f>'n = 15'!$U$41:$U$50</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1458,7 +1643,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'n = 15'!$V$41:$V$50</c:f>
+              <c:f>'n = 15'!$X$41:$X$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1889,7 +2074,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'n = 15'!$T$1</c:f>
+              <c:f>'n = 15'!$V$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1908,60 +2093,135 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-0376-4A87-A435-FE60DA772598}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-0376-4A87-A435-FE60DA772598}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-0376-4A87-A435-FE60DA772598}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'n = 15'!$S$2:$S$8</c:f>
+              <c:f>'n = 15'!$U$2:$U$11</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>full_10_2</c:v>
+                  <c:v>line_5_4 (15)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>grid_4_5</c:v>
+                  <c:v>full_10_2 (15)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>grid_9_3</c:v>
+                  <c:v>full_7_3 (8)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>line_5_4</c:v>
+                  <c:v>grid_9_3 (15)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>ring_10_2</c:v>
+                  <c:v>grid_4_5 (15)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>t_horizontal_5_4</c:v>
+                  <c:v>ring_10_2 (15)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>t_vertical_4</c:v>
+                  <c:v>ring_7_3 (8)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ring_5_4 (6)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>t_horizontal_5_4 (15)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>t_vertical_5_4 (15)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'n = 15'!$T$2:$T$8</c:f>
+              <c:f>'n = 15'!$V$2:$V$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>75.497499999999988</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>41.715833333333329</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>48.480000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.486666666666661</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
                   <c:v>36.87533333333333</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>30.486666666666661</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>75.497499999999988</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>62.43333333333333</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>38.339999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32.396666666666668</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>51.765999999999998</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>52.697999999999993</c:v>
                 </c:pt>
               </c:numCache>
@@ -1978,7 +2238,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'n = 15'!$U$1</c:f>
+              <c:f>'n = 15'!$W$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1997,60 +2257,135 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-0376-4A87-A435-FE60DA772598}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-0376-4A87-A435-FE60DA772598}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-0376-4A87-A435-FE60DA772598}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'n = 15'!$S$2:$S$8</c:f>
+              <c:f>'n = 15'!$U$2:$U$11</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>full_10_2</c:v>
+                  <c:v>line_5_4 (15)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>grid_4_5</c:v>
+                  <c:v>full_10_2 (15)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>grid_9_3</c:v>
+                  <c:v>full_7_3 (8)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>line_5_4</c:v>
+                  <c:v>grid_9_3 (15)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>ring_10_2</c:v>
+                  <c:v>grid_4_5 (15)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>t_horizontal_5_4</c:v>
+                  <c:v>ring_10_2 (15)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>t_vertical_4</c:v>
+                  <c:v>ring_7_3 (8)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ring_5_4 (6)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>t_horizontal_5_4 (15)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>t_vertical_5_4 (15)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'n = 15'!$U$2:$U$8</c:f>
+              <c:f>'n = 15'!$W$2:$W$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>-53.86</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>-203.42799999999997</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>-57.885000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-162.52799999999999</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
                   <c:v>-229.76733333333331</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>-162.52799999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-53.86</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>-200.90333333333334</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>-259.71500000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-120.74166666666667</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>-116.61466666666666</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>-116.79666666666665</c:v>
                 </c:pt>
               </c:numCache>
@@ -2177,8 +2512,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.11986466892218463"/>
-              <c:y val="0.31338684162788005"/>
+              <c:x val="8.2155789064006904E-2"/>
+              <c:y val="0.31338676339715488"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2330,10 +2665,13 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent4"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -3958,13 +4296,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>384174</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>165099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>42</xdr:col>
+      <xdr:col>44</xdr:col>
       <xdr:colOff>31750</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
@@ -3994,13 +4332,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>9524</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>577850</xdr:colOff>
       <xdr:row>76</xdr:row>
       <xdr:rowOff>10796</xdr:rowOff>
@@ -4030,14 +4368,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>122117</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>177799</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>314326</xdr:colOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>314328</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -4352,15 +4690,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Y147"/>
+  <dimension ref="A1:AC147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z41" sqref="Z41"/>
+    <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AJ9" sqref="AJ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1"/>
@@ -4372,15 +4711,17 @@
     <col min="14" max="14" width="15.1796875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.08984375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.81640625" customWidth="1"/>
-    <col min="24" max="24" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="11.81640625" customWidth="1"/>
+    <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.81640625" customWidth="1"/>
+    <col min="25" max="25" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4411,7 +4752,9 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="K1" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
@@ -4427,30 +4770,35 @@
       <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="T1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AC1" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -4496,33 +4844,39 @@
       <c r="P2">
         <v>15</v>
       </c>
-      <c r="R2">
-        <v>15</v>
-      </c>
-      <c r="S2" t="s">
-        <v>15</v>
-      </c>
-      <c r="T2" s="6">
-        <f>$I$17</f>
-        <v>41.715833333333329</v>
-      </c>
-      <c r="U2" s="6">
-        <f>$J$17</f>
-        <v>-203.42799999999997</v>
-      </c>
-      <c r="W2" t="s">
-        <v>15</v>
-      </c>
-      <c r="X2" s="2">
-        <f>$O$17</f>
-        <v>53.36933333333333</v>
-      </c>
-      <c r="Y2" s="5">
-        <f>$P$17</f>
-        <v>27.371999999999996</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="S2">
+        <v>15</v>
+      </c>
+      <c r="T2" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" t="str">
+        <f>T2 &amp; " (" &amp; S2 &amp; ")"</f>
+        <v>line_5_4 (15)</v>
+      </c>
+      <c r="V2" s="6">
+        <v>75.497499999999988</v>
+      </c>
+      <c r="W2" s="6">
+        <v>-53.86</v>
+      </c>
+      <c r="Y2" t="str">
+        <f t="shared" ref="Y2:Y11" si="0">U2</f>
+        <v>line_5_4 (15)</v>
+      </c>
+      <c r="Z2" s="2">
+        <f t="shared" ref="Z2:AA2" si="1">O78</f>
+        <v>61.018666666666668</v>
+      </c>
+      <c r="AA2" s="2">
+        <f t="shared" si="1"/>
+        <v>34.147333333333336</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4568,31 +4922,41 @@
       <c r="P3">
         <v>12.12</v>
       </c>
-      <c r="R3">
-        <v>15</v>
-      </c>
-      <c r="S3" t="s">
-        <v>33</v>
-      </c>
-      <c r="T3" s="6">
-        <f>$I$44</f>
-        <v>36.87533333333333</v>
-      </c>
-      <c r="U3" s="6">
-        <f>$J$44</f>
-        <v>-229.76733333333331</v>
-      </c>
-      <c r="W3" t="s">
-        <v>33</v>
-      </c>
-      <c r="X3" s="2">
-        <v>66.805999999999997</v>
-      </c>
-      <c r="Y3" s="2">
-        <v>28.262666666666668</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="S3">
+        <v>15</v>
+      </c>
+      <c r="T3" t="s">
+        <v>15</v>
+      </c>
+      <c r="U3" t="str">
+        <f>T3 &amp; " (" &amp; S3 &amp; ")"</f>
+        <v>full_10_2 (15)</v>
+      </c>
+      <c r="V3" s="6">
+        <f t="shared" ref="V3:W3" si="2">I17</f>
+        <v>41.715833333333329</v>
+      </c>
+      <c r="W3" s="6">
+        <f t="shared" si="2"/>
+        <v>-203.42799999999997</v>
+      </c>
+      <c r="Y3" t="str">
+        <f t="shared" si="0"/>
+        <v>full_10_2 (15)</v>
+      </c>
+      <c r="Z3" s="5">
+        <f t="shared" ref="Z3:AA3" si="3">O17</f>
+        <v>53.36933333333333</v>
+      </c>
+      <c r="AA3" s="5">
+        <f t="shared" si="3"/>
+        <v>27.371999999999996</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -4638,29 +5002,41 @@
       <c r="P4">
         <v>15</v>
       </c>
-      <c r="R4">
-        <v>15</v>
-      </c>
-      <c r="S4" t="s">
-        <v>34</v>
-      </c>
-      <c r="T4" s="6">
-        <v>30.486666666666661</v>
-      </c>
-      <c r="U4" s="6">
-        <v>-162.52799999999999</v>
-      </c>
-      <c r="W4" t="s">
-        <v>34</v>
-      </c>
-      <c r="X4" s="2">
-        <v>65.397999999999996</v>
-      </c>
-      <c r="Y4" s="2">
-        <v>26.140666666666668</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="S4">
+        <v>8</v>
+      </c>
+      <c r="T4" t="s">
+        <v>32</v>
+      </c>
+      <c r="U4" t="str">
+        <f>T4 &amp; " (" &amp; S4 &amp; ")"</f>
+        <v>full_7_3 (8)</v>
+      </c>
+      <c r="V4" s="7">
+        <f t="shared" ref="V4:W4" si="4">I27</f>
+        <v>48.480000000000004</v>
+      </c>
+      <c r="W4" s="7">
+        <f t="shared" si="4"/>
+        <v>-57.885000000000005</v>
+      </c>
+      <c r="Y4" t="str">
+        <f t="shared" si="0"/>
+        <v>full_7_3 (8)</v>
+      </c>
+      <c r="Z4" s="2">
+        <f t="shared" ref="Z4:AA4" si="5">O27</f>
+        <v>41.216250000000002</v>
+      </c>
+      <c r="AA4" s="2">
+        <f t="shared" si="5"/>
+        <v>19.568750000000001</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -4706,29 +5082,37 @@
       <c r="P5">
         <v>24.39</v>
       </c>
-      <c r="R5">
-        <v>15</v>
-      </c>
-      <c r="S5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T5" s="6">
-        <v>75.497499999999988</v>
-      </c>
-      <c r="U5" s="6">
-        <v>-53.86</v>
-      </c>
-      <c r="W5" t="s">
-        <v>35</v>
-      </c>
-      <c r="X5" s="2">
-        <v>61.018666666666668</v>
-      </c>
-      <c r="Y5" s="2">
-        <v>34.147333333333336</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="S5">
+        <v>15</v>
+      </c>
+      <c r="T5" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" t="str">
+        <f>T5 &amp; " (" &amp; S5 &amp; ")"</f>
+        <v>grid_9_3 (15)</v>
+      </c>
+      <c r="V5" s="6">
+        <v>30.486666666666661</v>
+      </c>
+      <c r="W5" s="6">
+        <v>-162.52799999999999</v>
+      </c>
+      <c r="Y5" t="str">
+        <f t="shared" si="0"/>
+        <v>grid_9_3 (15)</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>65.397999999999996</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>26.140666666666668</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -4774,29 +5158,41 @@
       <c r="P6">
         <v>4.26</v>
       </c>
-      <c r="R6">
-        <v>15</v>
-      </c>
-      <c r="S6" t="s">
-        <v>36</v>
-      </c>
-      <c r="T6" s="6">
-        <v>62.43333333333333</v>
-      </c>
-      <c r="U6" s="6">
-        <v>-200.90333333333334</v>
-      </c>
-      <c r="W6" t="s">
-        <v>36</v>
-      </c>
-      <c r="X6" s="2">
-        <v>48.56733333333333</v>
-      </c>
-      <c r="Y6" s="2">
-        <v>30.424666666666667</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="S6">
+        <v>15</v>
+      </c>
+      <c r="T6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U6" t="str">
+        <f>T6 &amp; " (" &amp; S6 &amp; ")"</f>
+        <v>grid_4_5 (15)</v>
+      </c>
+      <c r="V6" s="5">
+        <f>I44</f>
+        <v>36.87533333333333</v>
+      </c>
+      <c r="W6" s="5">
+        <f>J44</f>
+        <v>-229.76733333333331</v>
+      </c>
+      <c r="Y6" t="str">
+        <f t="shared" si="0"/>
+        <v>grid_4_5 (15)</v>
+      </c>
+      <c r="Z6" s="2">
+        <f t="shared" ref="Z6:AA6" si="6">O44</f>
+        <v>66.805999999999997</v>
+      </c>
+      <c r="AA6" s="2">
+        <f t="shared" si="6"/>
+        <v>28.262666666666668</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -4842,31 +5238,37 @@
       <c r="P7">
         <v>-30</v>
       </c>
-      <c r="R7">
-        <v>15</v>
-      </c>
-      <c r="S7" t="s">
-        <v>39</v>
-      </c>
-      <c r="T7" s="6">
-        <v>51.765999999999998</v>
-      </c>
-      <c r="U7" s="6">
-        <v>-116.61466666666666</v>
-      </c>
-      <c r="W7" t="s">
-        <v>39</v>
-      </c>
-      <c r="X7" s="2">
-        <f>$O$130</f>
-        <v>69.309333333333328</v>
-      </c>
-      <c r="Y7" s="2">
-        <f>$P$130</f>
-        <v>28.018666666666665</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="S7">
+        <v>15</v>
+      </c>
+      <c r="T7" t="s">
+        <v>36</v>
+      </c>
+      <c r="U7" t="str">
+        <f t="shared" ref="U3:U11" si="7">T7 &amp; " (" &amp; S7 &amp; ")"</f>
+        <v>ring_10_2 (15)</v>
+      </c>
+      <c r="V7" s="6">
+        <v>62.43333333333333</v>
+      </c>
+      <c r="W7" s="6">
+        <v>-200.90333333333334</v>
+      </c>
+      <c r="Y7" t="str">
+        <f t="shared" si="0"/>
+        <v>ring_10_2 (15)</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>48.56733333333333</v>
+      </c>
+      <c r="AA7" s="2">
+        <v>30.424666666666667</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -4912,184 +5314,259 @@
       <c r="P8">
         <v>21.5</v>
       </c>
-      <c r="R8">
-        <v>15</v>
-      </c>
-      <c r="S8" t="s">
-        <v>42</v>
-      </c>
-      <c r="T8" s="6">
+      <c r="S8">
+        <v>8</v>
+      </c>
+      <c r="T8" t="s">
+        <v>38</v>
+      </c>
+      <c r="U8" t="str">
+        <f t="shared" si="7"/>
+        <v>ring_7_3 (8)</v>
+      </c>
+      <c r="V8" s="7">
+        <v>38.339999999999996</v>
+      </c>
+      <c r="W8" s="7">
+        <v>-259.71500000000003</v>
+      </c>
+      <c r="Y8" t="str">
+        <f t="shared" si="0"/>
+        <v>ring_7_3 (8)</v>
+      </c>
+      <c r="Z8" s="2">
+        <f>$O$113</f>
+        <v>33.421250000000001</v>
+      </c>
+      <c r="AA8" s="2">
+        <f>$P$113</f>
+        <v>32.08</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>608</v>
+      </c>
+      <c r="E9">
+        <v>122</v>
+      </c>
+      <c r="F9">
+        <v>378</v>
+      </c>
+      <c r="G9">
+        <v>72</v>
+      </c>
+      <c r="H9">
+        <v>321</v>
+      </c>
+      <c r="I9">
+        <v>15.08</v>
+      </c>
+      <c r="J9">
+        <v>-345.83</v>
+      </c>
+      <c r="L9">
+        <v>489</v>
+      </c>
+      <c r="M9">
+        <v>329</v>
+      </c>
+      <c r="N9">
+        <v>245</v>
+      </c>
+      <c r="O9">
+        <v>49.9</v>
+      </c>
+      <c r="P9">
+        <v>25.53</v>
+      </c>
+      <c r="S9">
+        <v>6</v>
+      </c>
+      <c r="T9" t="s">
+        <v>37</v>
+      </c>
+      <c r="U9" t="str">
+        <f t="shared" si="7"/>
+        <v>ring_5_4 (6)</v>
+      </c>
+      <c r="V9" s="7">
+        <v>32.396666666666668</v>
+      </c>
+      <c r="W9" s="7">
+        <v>-120.74166666666667</v>
+      </c>
+      <c r="Y9" t="str">
+        <f t="shared" si="0"/>
+        <v>ring_5_4 (6)</v>
+      </c>
+      <c r="Z9" s="2">
+        <v>22.03833333333333</v>
+      </c>
+      <c r="AA9" s="2">
+        <v>38.961666666666666</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>615</v>
+      </c>
+      <c r="E10">
+        <v>77</v>
+      </c>
+      <c r="F10">
+        <v>1146</v>
+      </c>
+      <c r="G10">
+        <v>177</v>
+      </c>
+      <c r="H10">
+        <v>315</v>
+      </c>
+      <c r="I10">
+        <v>72.510000000000005</v>
+      </c>
+      <c r="J10">
+        <v>-77.97</v>
+      </c>
+      <c r="L10">
+        <v>1399</v>
+      </c>
+      <c r="M10">
+        <v>372</v>
+      </c>
+      <c r="N10">
+        <v>210</v>
+      </c>
+      <c r="O10">
+        <v>84.99</v>
+      </c>
+      <c r="P10">
+        <v>43.55</v>
+      </c>
+      <c r="S10">
+        <v>15</v>
+      </c>
+      <c r="T10" t="s">
+        <v>39</v>
+      </c>
+      <c r="U10" t="str">
+        <f t="shared" si="7"/>
+        <v>t_horizontal_5_4 (15)</v>
+      </c>
+      <c r="V10" s="6">
+        <v>51.765999999999998</v>
+      </c>
+      <c r="W10" s="6">
+        <v>-116.61466666666666</v>
+      </c>
+      <c r="Y10" t="str">
+        <f t="shared" si="0"/>
+        <v>t_horizontal_5_4 (15)</v>
+      </c>
+      <c r="Z10" s="2">
+        <f t="shared" ref="Z10:AA10" si="8">O130</f>
+        <v>69.309333333333328</v>
+      </c>
+      <c r="AA10" s="2">
+        <f t="shared" si="8"/>
+        <v>28.018666666666665</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>615</v>
+      </c>
+      <c r="E11">
+        <v>77</v>
+      </c>
+      <c r="F11">
+        <v>1146</v>
+      </c>
+      <c r="G11">
+        <v>138</v>
+      </c>
+      <c r="H11">
+        <v>315</v>
+      </c>
+      <c r="I11">
+        <v>72.510000000000005</v>
+      </c>
+      <c r="J11">
+        <v>-128.26</v>
+      </c>
+      <c r="L11">
+        <v>1399</v>
+      </c>
+      <c r="M11">
+        <v>327</v>
+      </c>
+      <c r="N11">
+        <v>210</v>
+      </c>
+      <c r="O11">
+        <v>84.99</v>
+      </c>
+      <c r="P11">
+        <v>35.78</v>
+      </c>
+      <c r="S11">
+        <v>15</v>
+      </c>
+      <c r="T11" t="s">
+        <v>40</v>
+      </c>
+      <c r="U11" t="str">
+        <f t="shared" si="7"/>
+        <v>t_vertical_5_4 (15)</v>
+      </c>
+      <c r="V11" s="6">
         <v>52.697999999999993</v>
       </c>
-      <c r="U8" s="6">
+      <c r="W11" s="6">
         <v>-116.79666666666665</v>
       </c>
-      <c r="W8" t="s">
-        <v>42</v>
-      </c>
-      <c r="X8" s="2">
+      <c r="Y11" t="str">
+        <f t="shared" si="0"/>
+        <v>t_vertical_5_4 (15)</v>
+      </c>
+      <c r="Z11" s="2">
         <f>$O$147</f>
         <v>70.554000000000002</v>
       </c>
-      <c r="Y8" s="2">
+      <c r="AA11" s="2">
         <f>$P$147</f>
         <v>32.405999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9">
-        <v>15</v>
-      </c>
-      <c r="D9">
-        <v>608</v>
-      </c>
-      <c r="E9">
-        <v>122</v>
-      </c>
-      <c r="F9">
-        <v>378</v>
-      </c>
-      <c r="G9">
-        <v>72</v>
-      </c>
-      <c r="H9">
-        <v>321</v>
-      </c>
-      <c r="I9">
-        <v>15.08</v>
-      </c>
-      <c r="J9">
-        <v>-345.83</v>
-      </c>
-      <c r="L9">
-        <v>489</v>
-      </c>
-      <c r="M9">
-        <v>329</v>
-      </c>
-      <c r="N9">
-        <v>245</v>
-      </c>
-      <c r="O9">
-        <v>49.9</v>
-      </c>
-      <c r="P9">
-        <v>25.53</v>
-      </c>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10">
-        <v>15</v>
-      </c>
-      <c r="D10">
-        <v>615</v>
-      </c>
-      <c r="E10">
-        <v>77</v>
-      </c>
-      <c r="F10">
-        <v>1146</v>
-      </c>
-      <c r="G10">
-        <v>177</v>
-      </c>
-      <c r="H10">
-        <v>315</v>
-      </c>
-      <c r="I10">
-        <v>72.510000000000005</v>
-      </c>
-      <c r="J10">
-        <v>-77.97</v>
-      </c>
-      <c r="L10">
-        <v>1399</v>
-      </c>
-      <c r="M10">
-        <v>372</v>
-      </c>
-      <c r="N10">
-        <v>210</v>
-      </c>
-      <c r="O10">
-        <v>84.99</v>
-      </c>
-      <c r="P10">
-        <v>43.55</v>
-      </c>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11">
-        <v>15</v>
-      </c>
-      <c r="D11">
-        <v>615</v>
-      </c>
-      <c r="E11">
-        <v>77</v>
-      </c>
-      <c r="F11">
-        <v>1146</v>
-      </c>
-      <c r="G11">
-        <v>138</v>
-      </c>
-      <c r="H11">
-        <v>315</v>
-      </c>
-      <c r="I11">
-        <v>72.510000000000005</v>
-      </c>
-      <c r="J11">
-        <v>-128.26</v>
-      </c>
-      <c r="L11">
-        <v>1399</v>
-      </c>
-      <c r="M11">
-        <v>327</v>
-      </c>
-      <c r="N11">
-        <v>210</v>
-      </c>
-      <c r="O11">
-        <v>84.99</v>
-      </c>
-      <c r="P11">
-        <v>35.78</v>
-      </c>
-      <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
-      <c r="X11" s="2"/>
-      <c r="Y11" s="2"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -5135,33 +5612,8 @@
       <c r="P12">
         <v>52.43</v>
       </c>
-      <c r="R12">
-        <v>8</v>
-      </c>
-      <c r="S12" t="s">
-        <v>32</v>
-      </c>
-      <c r="T12" s="8">
-        <f>$I$27</f>
-        <v>48.480000000000004</v>
-      </c>
-      <c r="U12" s="8">
-        <f>$J$27</f>
-        <v>-57.885000000000005</v>
-      </c>
-      <c r="W12" t="s">
-        <v>32</v>
-      </c>
-      <c r="X12" s="2">
-        <f>$O$27</f>
-        <v>41.216250000000002</v>
-      </c>
-      <c r="Y12" s="2">
-        <f>$P$27</f>
-        <v>19.568750000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -5207,29 +5659,8 @@
       <c r="P13">
         <v>42.69</v>
       </c>
-      <c r="R13">
-        <v>6</v>
-      </c>
-      <c r="S13" t="s">
-        <v>37</v>
-      </c>
-      <c r="T13" s="8">
-        <v>32.396666666666668</v>
-      </c>
-      <c r="U13" s="8">
-        <v>-120.74166666666667</v>
-      </c>
-      <c r="W13" t="s">
-        <v>37</v>
-      </c>
-      <c r="X13" s="2">
-        <v>22.03833333333333</v>
-      </c>
-      <c r="Y13" s="2">
-        <v>38.961666666666666</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -5275,31 +5706,8 @@
       <c r="P14">
         <v>54.83</v>
       </c>
-      <c r="R14">
-        <v>8</v>
-      </c>
-      <c r="S14" t="s">
-        <v>38</v>
-      </c>
-      <c r="T14" s="8">
-        <v>38.339999999999996</v>
-      </c>
-      <c r="U14" s="8">
-        <v>-259.71500000000003</v>
-      </c>
-      <c r="W14" t="s">
-        <v>38</v>
-      </c>
-      <c r="X14" s="2">
-        <f>$O$113</f>
-        <v>33.421250000000001</v>
-      </c>
-      <c r="Y14" s="2">
-        <f>$P$113</f>
-        <v>32.08</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -5346,7 +5754,7 @@
         <v>44.72</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -5393,7 +5801,7 @@
         <v>48.78</v>
       </c>
     </row>
-    <row r="17" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -5417,12 +5825,12 @@
         <f>AVERAGE(P2:P16)</f>
         <v>27.371999999999996</v>
       </c>
-      <c r="V17"/>
-    </row>
-    <row r="18" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="V18"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="X17"/>
+    </row>
+    <row r="18" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="X18"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -5469,7 +5877,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -5516,7 +5924,7 @@
         <v>16.670000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -5563,7 +5971,7 @@
         <v>8.57</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -5610,7 +6018,7 @@
         <v>44.64</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -5657,7 +6065,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -5704,7 +6112,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -5751,7 +6159,7 @@
         <v>27.8</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -5798,7 +6206,7 @@
         <v>45.61</v>
       </c>
     </row>
-    <row r="27" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>32</v>
       </c>
@@ -5822,9 +6230,9 @@
         <f>AVERAGE(P19:P26)</f>
         <v>19.568750000000001</v>
       </c>
-      <c r="V27"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="X27"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -5871,7 +6279,7 @@
         <v>21.88</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -5918,7 +6326,7 @@
         <v>49.33</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -5965,7 +6373,7 @@
         <v>-22.58</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -6012,7 +6420,7 @@
         <v>18.329999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -6059,7 +6467,7 @@
         <v>26.09</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -6106,7 +6514,7 @@
         <v>-20.69</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -6153,7 +6561,7 @@
         <v>33.950000000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -6200,7 +6608,7 @@
         <v>29.21</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -6247,7 +6655,7 @@
         <v>51.94</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -6294,7 +6702,7 @@
         <v>55.61</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -6341,7 +6749,7 @@
         <v>52.13</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -6387,20 +6795,20 @@
       <c r="P40">
         <v>14.25</v>
       </c>
-      <c r="S40" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="T40" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="U40" s="9" t="s">
+      <c r="U40" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="V40" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="V40" s="9" t="s">
+      <c r="W40" s="8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="X40" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -6446,24 +6854,24 @@
       <c r="P41">
         <v>28.55</v>
       </c>
-      <c r="S41" t="str">
-        <f t="shared" ref="S41" si="0">A17</f>
+      <c r="U41" t="str">
+        <f t="shared" ref="U41" si="9">A17</f>
         <v>full_10_2</v>
       </c>
-      <c r="T41">
+      <c r="V41">
         <f>'n = 5'!$B$17</f>
         <v>15</v>
       </c>
-      <c r="U41">
+      <c r="W41">
         <f>'n = 10'!$B$17</f>
         <v>15</v>
       </c>
-      <c r="V41">
+      <c r="X41">
         <f>B17</f>
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>33</v>
       </c>
@@ -6509,24 +6917,24 @@
       <c r="P42">
         <v>40.44</v>
       </c>
-      <c r="S42" t="str">
-        <f t="shared" ref="S42" si="1">A27</f>
+      <c r="U42" t="str">
+        <f t="shared" ref="U42" si="10">A27</f>
         <v>full_7_3</v>
       </c>
-      <c r="T42">
+      <c r="V42">
         <f>'n = 5'!$B$33</f>
         <v>15</v>
       </c>
-      <c r="U42">
+      <c r="W42">
         <f>'n = 10'!$B$33</f>
         <v>15</v>
       </c>
-      <c r="V42">
+      <c r="X42">
         <f>B27</f>
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -6572,24 +6980,24 @@
       <c r="P43">
         <v>45.5</v>
       </c>
-      <c r="S43" t="str">
-        <f t="shared" ref="S43" si="2">A44</f>
+      <c r="U43" t="str">
+        <f t="shared" ref="U43" si="11">A44</f>
         <v>grid_4_5</v>
       </c>
-      <c r="T43">
+      <c r="V43">
         <f>'n = 5'!$B$49</f>
         <v>15</v>
       </c>
-      <c r="U43">
+      <c r="W43">
         <f>'n = 10'!$B$49</f>
         <v>15</v>
       </c>
-      <c r="V43">
+      <c r="X43">
         <f>B44</f>
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>33</v>
       </c>
@@ -6597,11 +7005,11 @@
         <f>COUNTA(B29:B43)</f>
         <v>15</v>
       </c>
-      <c r="I44" s="3">
+      <c r="I44" s="5">
         <f>AVERAGE(I29:I43)</f>
         <v>36.87533333333333</v>
       </c>
-      <c r="J44" s="3">
+      <c r="J44" s="5">
         <f>AVERAGE(J29:J43)</f>
         <v>-229.76733333333331</v>
       </c>
@@ -6613,42 +7021,42 @@
         <f>AVERAGE(P29:P43)</f>
         <v>28.262666666666668</v>
       </c>
-      <c r="S44" s="3" t="str">
-        <f t="shared" ref="S44" si="3">A61</f>
+      <c r="U44" s="3" t="str">
+        <f t="shared" ref="U44" si="12">A61</f>
         <v>grid_9_3</v>
       </c>
-      <c r="T44">
+      <c r="V44">
         <f>'n = 5'!$B$65</f>
         <v>15</v>
       </c>
-      <c r="U44" s="3">
+      <c r="W44" s="3">
         <f>'n = 10'!$B$65</f>
         <v>15</v>
       </c>
-      <c r="V44" s="3">
+      <c r="X44" s="3">
         <f>B61</f>
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="S45" t="str">
-        <f t="shared" ref="S45" si="4">A78</f>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="U45" t="str">
+        <f t="shared" ref="U45" si="13">A78</f>
         <v>line_5_4</v>
       </c>
-      <c r="T45">
+      <c r="V45">
         <f>'n = 5'!$B$81</f>
         <v>15</v>
       </c>
-      <c r="U45">
+      <c r="W45">
         <f>'n = 10'!$B$81</f>
         <v>15</v>
       </c>
-      <c r="V45">
+      <c r="X45">
         <f>B78</f>
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>34</v>
       </c>
@@ -6694,23 +7102,23 @@
       <c r="P46">
         <v>-25</v>
       </c>
-      <c r="S46" t="str">
-        <f t="shared" ref="S46" si="5">A95</f>
+      <c r="U46" t="str">
+        <f t="shared" ref="U46" si="14">A95</f>
         <v>ring_10_2</v>
       </c>
-      <c r="T46">
+      <c r="V46">
         <f>'n = 5'!$B$97</f>
         <v>15</v>
       </c>
-      <c r="U46">
-        <v>15</v>
-      </c>
-      <c r="V46">
+      <c r="W46">
+        <v>15</v>
+      </c>
+      <c r="X46">
         <f>B95</f>
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>34</v>
       </c>
@@ -6756,24 +7164,24 @@
       <c r="P47">
         <v>49.25</v>
       </c>
-      <c r="S47" t="str">
-        <f t="shared" ref="S47" si="6">A103</f>
+      <c r="U47" t="str">
+        <f t="shared" ref="U47" si="15">A103</f>
         <v>ring_5_4</v>
       </c>
-      <c r="T47">
+      <c r="V47">
         <f>'n = 5'!$B$108</f>
         <v>10</v>
       </c>
-      <c r="U47">
+      <c r="W47">
         <f>'n = 10'!$B$105</f>
         <v>7</v>
       </c>
-      <c r="V47">
+      <c r="X47">
         <f>B103</f>
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>34</v>
       </c>
@@ -6819,23 +7227,23 @@
       <c r="P48">
         <v>13.16</v>
       </c>
-      <c r="S48" t="str">
-        <f t="shared" ref="S48" si="7">A113</f>
+      <c r="U48" t="str">
+        <f t="shared" ref="U48" si="16">A113</f>
         <v>ring_7_3</v>
       </c>
-      <c r="T48">
+      <c r="V48">
         <f>'n = 5'!$B$124</f>
         <v>15</v>
       </c>
-      <c r="U48">
+      <c r="W48">
         <v>10</v>
       </c>
-      <c r="V48">
+      <c r="X48">
         <f>B113</f>
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>34</v>
       </c>
@@ -6881,24 +7289,24 @@
       <c r="P49">
         <v>-4.4400000000000004</v>
       </c>
-      <c r="S49" t="str">
-        <f t="shared" ref="S49" si="8">A130</f>
+      <c r="U49" t="str">
+        <f t="shared" ref="U49" si="17">A130</f>
         <v>t_horizontal_5_4</v>
       </c>
-      <c r="T49">
+      <c r="V49">
         <f>'n = 5'!$B$140</f>
         <v>15</v>
       </c>
-      <c r="U49">
+      <c r="W49">
         <f>'n = 10'!$B$132</f>
         <v>15</v>
       </c>
-      <c r="V49">
+      <c r="X49">
         <f>B130</f>
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>34</v>
       </c>
@@ -6944,24 +7352,24 @@
       <c r="P50">
         <v>27.21</v>
       </c>
-      <c r="S50" t="str">
-        <f t="shared" ref="S50" si="9">A147</f>
+      <c r="U50" t="str">
+        <f t="shared" ref="U50" si="18">A147</f>
         <v>t_vertical_5_4</v>
       </c>
-      <c r="T50" s="3">
+      <c r="V50" s="3">
         <f>'n = 5'!$B$156</f>
         <v>15</v>
       </c>
-      <c r="U50">
+      <c r="W50">
         <f>'n = 10'!$B$148</f>
         <v>15</v>
       </c>
-      <c r="V50">
+      <c r="X50">
         <f>B147</f>
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>34</v>
       </c>
@@ -7008,7 +7416,7 @@
         <v>-39.22</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>34</v>
       </c>
@@ -7055,7 +7463,7 @@
         <v>30.48</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>34</v>
       </c>
@@ -7102,7 +7510,7 @@
         <v>41.28</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>34</v>
       </c>
@@ -7149,7 +7557,7 @@
         <v>45.33</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>34</v>
       </c>
@@ -7196,7 +7604,7 @@
         <v>47.02</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>34</v>
       </c>
@@ -7243,7 +7651,7 @@
         <v>50.51</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>34</v>
       </c>
@@ -7290,7 +7698,7 @@
         <v>24.78</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>34</v>
       </c>
@@ -7337,7 +7745,7 @@
         <v>37.1</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>34</v>
       </c>
@@ -7384,7 +7792,7 @@
         <v>51.06</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>34</v>
       </c>
@@ -7431,7 +7839,7 @@
         <v>43.59</v>
       </c>
     </row>
-    <row r="61" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>34</v>
       </c>
@@ -7455,9 +7863,9 @@
         <f>AVERAGE(P46:P60)</f>
         <v>26.140666666666668</v>
       </c>
-      <c r="V61"/>
-    </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="X61"/>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>35</v>
       </c>
@@ -7504,7 +7912,7 @@
         <v>13.04</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>35</v>
       </c>
@@ -7551,7 +7959,7 @@
         <v>55.88</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>35</v>
       </c>
@@ -7598,7 +8006,7 @@
         <v>-48.48</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>35</v>
       </c>
@@ -7645,7 +8053,7 @@
         <v>48.19</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>35</v>
       </c>
@@ -7692,7 +8100,7 @@
         <v>10.37</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>35</v>
       </c>
@@ -7739,7 +8147,7 @@
         <v>-26.79</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>35</v>
       </c>
@@ -7786,7 +8194,7 @@
         <v>46.2</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>35</v>
       </c>
@@ -7833,7 +8241,7 @@
         <v>43.09</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>35</v>
       </c>
@@ -7880,7 +8288,7 @@
         <v>61.24</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>35</v>
       </c>
@@ -7927,7 +8335,7 @@
         <v>61.06</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>35</v>
       </c>
@@ -7974,7 +8382,7 @@
         <v>64.209999999999994</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>35</v>
       </c>
@@ -8021,7 +8429,7 @@
         <v>45.71</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>35</v>
       </c>
@@ -8068,7 +8476,7 @@
         <v>51.04</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>35</v>
       </c>
@@ -8115,7 +8523,7 @@
         <v>41.84</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>35</v>
       </c>
@@ -8162,7 +8570,7 @@
         <v>45.61</v>
       </c>
     </row>
-    <row r="78" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>35</v>
       </c>
@@ -8186,9 +8594,9 @@
         <f>AVERAGE(P63:P77)</f>
         <v>34.147333333333336</v>
       </c>
-      <c r="V78"/>
-    </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="X78"/>
+    </row>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>36</v>
       </c>
@@ -8235,7 +8643,7 @@
         <v>-53.85</v>
       </c>
     </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>36</v>
       </c>
@@ -8282,7 +8690,7 @@
         <v>60.56</v>
       </c>
     </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>36</v>
       </c>
@@ -8329,7 +8737,7 @@
         <v>3.12</v>
       </c>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>36</v>
       </c>
@@ -8376,7 +8784,7 @@
         <v>6.35</v>
       </c>
     </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>36</v>
       </c>
@@ -8423,7 +8831,7 @@
         <v>43.48</v>
       </c>
     </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>36</v>
       </c>
@@ -8470,7 +8878,7 @@
         <v>-11.11</v>
       </c>
     </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>36</v>
       </c>
@@ -8517,7 +8925,7 @@
         <v>52.19</v>
       </c>
     </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>36</v>
       </c>
@@ -8564,7 +8972,7 @@
         <v>37.21</v>
       </c>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>36</v>
       </c>
@@ -8611,7 +9019,7 @@
         <v>46.55</v>
       </c>
     </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>36</v>
       </c>
@@ -8658,7 +9066,7 @@
         <v>49.75</v>
       </c>
     </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>36</v>
       </c>
@@ -8705,7 +9113,7 @@
         <v>53.86</v>
       </c>
     </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>36</v>
       </c>
@@ -8752,7 +9160,7 @@
         <v>37.46</v>
       </c>
     </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>36</v>
       </c>
@@ -8799,7 +9207,7 @@
         <v>32.659999999999997</v>
       </c>
     </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>36</v>
       </c>
@@ -8846,7 +9254,7 @@
         <v>48.63</v>
       </c>
     </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>36</v>
       </c>
@@ -8893,7 +9301,7 @@
         <v>49.51</v>
       </c>
     </row>
-    <row r="95" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
         <v>36</v>
       </c>
@@ -8917,9 +9325,9 @@
         <f>AVERAGE(P80:P94)</f>
         <v>30.424666666666667</v>
       </c>
-      <c r="V95"/>
-    </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="X95"/>
+    </row>
+    <row r="97" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>37</v>
       </c>
@@ -8966,7 +9374,7 @@
         <v>26.83</v>
       </c>
     </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>37</v>
       </c>
@@ -9013,7 +9421,7 @@
         <v>53.52</v>
       </c>
     </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>37</v>
       </c>
@@ -9060,7 +9468,7 @@
         <v>15.79</v>
       </c>
     </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>37</v>
       </c>
@@ -9107,7 +9515,7 @@
         <v>42.11</v>
       </c>
     </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>37</v>
       </c>
@@ -9154,7 +9562,7 @@
         <v>47.33</v>
       </c>
     </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>37</v>
       </c>
@@ -9201,7 +9609,7 @@
         <v>48.19</v>
       </c>
     </row>
-    <row r="103" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
         <v>37</v>
       </c>
@@ -9218,16 +9626,16 @@
         <v>-120.74166666666667</v>
       </c>
       <c r="O103" s="3">
-        <f t="shared" ref="O103:P103" si="10">AVERAGE(O97:O102)</f>
+        <f t="shared" ref="O103:P103" si="19">AVERAGE(O97:O102)</f>
         <v>22.03833333333333</v>
       </c>
       <c r="P103" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>38.961666666666666</v>
       </c>
-      <c r="V103"/>
-    </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="X103"/>
+    </row>
+    <row r="105" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>38</v>
       </c>
@@ -9274,7 +9682,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="106" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>38</v>
       </c>
@@ -9321,7 +9729,7 @@
         <v>56.06</v>
       </c>
     </row>
-    <row r="107" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>38</v>
       </c>
@@ -9368,7 +9776,7 @@
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>38</v>
       </c>
@@ -9415,7 +9823,7 @@
         <v>15.87</v>
       </c>
     </row>
-    <row r="109" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>38</v>
       </c>
@@ -9462,7 +9870,7 @@
         <v>43.75</v>
       </c>
     </row>
-    <row r="110" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>38</v>
       </c>
@@ -9509,7 +9917,7 @@
         <v>6.58</v>
       </c>
     </row>
-    <row r="111" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>38</v>
       </c>
@@ -9556,7 +9964,7 @@
         <v>56.89</v>
       </c>
     </row>
-    <row r="112" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>38</v>
       </c>
@@ -9603,7 +10011,7 @@
         <v>46.39</v>
       </c>
     </row>
-    <row r="113" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A113" s="3" t="s">
         <v>38</v>
       </c>
@@ -9627,9 +10035,9 @@
         <f>AVERAGE(P105:P112)</f>
         <v>32.08</v>
       </c>
-      <c r="V113"/>
-    </row>
-    <row r="115" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="X113"/>
+    </row>
+    <row r="115" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>39</v>
       </c>
@@ -9676,7 +10084,7 @@
         <v>47.17</v>
       </c>
     </row>
-    <row r="116" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>39</v>
       </c>
@@ -9723,7 +10131,7 @@
         <v>38.46</v>
       </c>
     </row>
-    <row r="117" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>39</v>
       </c>
@@ -9770,7 +10178,7 @@
         <v>-21.62</v>
       </c>
     </row>
-    <row r="118" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>39</v>
       </c>
@@ -9817,7 +10225,7 @@
         <v>-38.24</v>
       </c>
     </row>
-    <row r="119" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>39</v>
       </c>
@@ -9864,7 +10272,7 @@
         <v>21.28</v>
       </c>
     </row>
-    <row r="120" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>39</v>
       </c>
@@ -9911,7 +10319,7 @@
         <v>-19.64</v>
       </c>
     </row>
-    <row r="121" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>39</v>
       </c>
@@ -9958,7 +10366,7 @@
         <v>44.98</v>
       </c>
     </row>
-    <row r="122" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>39</v>
       </c>
@@ -10005,7 +10413,7 @@
         <v>44.69</v>
       </c>
     </row>
-    <row r="123" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>39</v>
       </c>
@@ -10052,7 +10460,7 @@
         <v>47.53</v>
       </c>
     </row>
-    <row r="124" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>39</v>
       </c>
@@ -10099,7 +10507,7 @@
         <v>44.81</v>
       </c>
     </row>
-    <row r="125" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>39</v>
       </c>
@@ -10146,7 +10554,7 @@
         <v>55.95</v>
       </c>
     </row>
-    <row r="126" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>39</v>
       </c>
@@ -10193,7 +10601,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="127" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>39</v>
       </c>
@@ -10240,7 +10648,7 @@
         <v>33.96</v>
       </c>
     </row>
-    <row r="128" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>39</v>
       </c>
@@ -10287,7 +10695,7 @@
         <v>43.01</v>
       </c>
     </row>
-    <row r="129" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>39</v>
       </c>
@@ -10334,7 +10742,7 @@
         <v>51.74</v>
       </c>
     </row>
-    <row r="130" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A130" s="3" t="s">
         <v>39</v>
       </c>
@@ -10358,9 +10766,9 @@
         <f>AVERAGE(P115:P129)</f>
         <v>28.018666666666665</v>
       </c>
-      <c r="V130"/>
-    </row>
-    <row r="132" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="X130"/>
+    </row>
+    <row r="132" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>40</v>
       </c>
@@ -10407,7 +10815,7 @@
         <v>50.85</v>
       </c>
     </row>
-    <row r="133" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>40</v>
       </c>
@@ -10454,7 +10862,7 @@
         <v>44.93</v>
       </c>
     </row>
-    <row r="134" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>40</v>
       </c>
@@ -10501,7 +10909,7 @@
         <v>-17.14</v>
       </c>
     </row>
-    <row r="135" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>40</v>
       </c>
@@ -10548,7 +10956,7 @@
         <v>11.11</v>
       </c>
     </row>
-    <row r="136" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>40</v>
       </c>
@@ -10595,7 +11003,7 @@
         <v>36.6</v>
       </c>
     </row>
-    <row r="137" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>40</v>
       </c>
@@ -10642,7 +11050,7 @@
         <v>-43.55</v>
       </c>
     </row>
-    <row r="138" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>40</v>
       </c>
@@ -10689,7 +11097,7 @@
         <v>36.93</v>
       </c>
     </row>
-    <row r="139" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>40</v>
       </c>
@@ -10736,7 +11144,7 @@
         <v>40.46</v>
       </c>
     </row>
-    <row r="140" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>40</v>
       </c>
@@ -10783,7 +11191,7 @@
         <v>53.72</v>
       </c>
     </row>
-    <row r="141" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>40</v>
       </c>
@@ -10830,7 +11238,7 @@
         <v>55.99</v>
       </c>
     </row>
-    <row r="142" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>40</v>
       </c>
@@ -10877,7 +11285,7 @@
         <v>59.73</v>
       </c>
     </row>
-    <row r="143" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>40</v>
       </c>
@@ -10924,7 +11332,7 @@
         <v>32.42</v>
       </c>
     </row>
-    <row r="144" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>40</v>
       </c>
@@ -10971,7 +11379,7 @@
         <v>32.92</v>
       </c>
     </row>
-    <row r="145" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>40</v>
       </c>
@@ -11018,7 +11426,7 @@
         <v>45.8</v>
       </c>
     </row>
-    <row r="146" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>40</v>
       </c>
@@ -11065,7 +11473,7 @@
         <v>45.32</v>
       </c>
     </row>
-    <row r="147" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A147" s="3" t="s">
         <v>40</v>
       </c>
@@ -11089,7 +11497,7 @@
         <f>AVERAGE(P132:P146)</f>
         <v>32.405999999999999</v>
       </c>
-      <c r="V147"/>
+      <c r="X147"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>